<commit_message>
Updated code of ooh pbt
</commit_message>
<xml_diff>
--- a/OOH_PBT/OOH_PBT_Performer/Data/Config.xlsx
+++ b/OOH_PBT/OOH_PBT_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Files\UPProjects\OOH_PBT\OOH_PBT_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E948075D-CC1B-4C62-A188-513276B46C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343250D-ED4A-48E9-9531-6522A9EF499A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,7 @@
     <t>ApdigitalUSA</t>
   </si>
   <si>
-    <t>C:\Users\NTMGRM.RPA1\Desktop\Exception Screenshots\</t>
+    <t>C:\Users\NTMGRM.RPA1\Desktop\OOH_PBT_Exception_Screenshots\</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>